<commit_message>
update excel template for import student and employee data
</commit_message>
<xml_diff>
--- a/api/public/template/TEMPLATE-IMPOR-PEGAWAI.xlsx
+++ b/api/public/template/TEMPLATE-IMPOR-PEGAWAI.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>nama</t>
   </si>
@@ -46,6 +46,9 @@
   <si>
     <t>telepon</t>
   </si>
+  <si>
+    <t>PERHATIAN: Kolom jenis pegawai hanya boleh diisi dengan PNS, PPPK atau HONORER</t>
+  </si>
 </sst>
 </file>
 
@@ -57,8 +60,16 @@
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20">
-    <font>
+  <fonts count="21">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -210,7 +221,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +231,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,55 +553,52 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -599,78 +613,84 @@
     <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -946,6 +966,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1206,17 +1233,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="21.7777777777778" customWidth="1"/>
     <col min="2" max="2" width="20.8888888888889" customWidth="1"/>
@@ -1224,9 +1251,10 @@
     <col min="4" max="4" width="13.5555555555556" customWidth="1"/>
     <col min="5" max="5" width="20.4444444444444" customWidth="1"/>
     <col min="6" max="6" width="14.1111111111111" customWidth="1"/>
+    <col min="7" max="7" width="73" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1245,9 +1273,33 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="4Z+73pVGbnZLK9EHNAhhsrtt9pu+lH+0vxAuxWJLmjdls+NNrjwzjyNtQOX/uaIs0hSnIx/uWOs9JA0LAJR4GA==" saltValue="RF3VB3ePSba58SLWQNsgGg==" spinCount="100000" sheet="1" objects="1"/>
+  <protectedRanges>
+    <protectedRange sqref="A2:F500" name="input data"/>
+  </protectedRanges>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<allowEditUser xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" hasInvisiblePropRange="0">
+  <rangeList sheetStid="1" master="" otherUserPermission="visible">
+    <arrUserId title="input data" rangeCreator="" othersAccessPermission="edit"/>
+  </rangeList>
+</allowEditUser>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A5607D9-04D2-4DE1-AC0E-A7772F01BC71}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>